<commit_message>
update hotel reviews data
</commit_message>
<xml_diff>
--- a/data/hotels_by_city/Denver/Denver_shard_130.xlsx
+++ b/data/hotels_by_city/Denver/Denver_shard_130.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="hotel_info" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="review_info" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="hotel_info" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="review_info" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="173">
   <si>
     <t>STR#</t>
   </si>
@@ -63,6 +63,12 @@
     <t>https://www.tripadvisor.com/Hotel_Review-g609128-d10190804-Reviews-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
   </si>
   <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>https://www.orbitz.com/Denver-Hotels-Holiday-Inn-Hotel-Suites-Denver-Tech-Center-Centennial.h15137712.Hotel-Information</t>
   </si>
   <si>
@@ -139,6 +145,396 @@
   </si>
   <si>
     <t>response_text</t>
+  </si>
+  <si>
+    <t>08/02/2018</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r595882257-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>609128</t>
+  </si>
+  <si>
+    <t>10190804</t>
+  </si>
+  <si>
+    <t>595882257</t>
+  </si>
+  <si>
+    <t>07/13/2018</t>
+  </si>
+  <si>
+    <t>So nice!</t>
+  </si>
+  <si>
+    <t>This is a beautiful facility well maintained by dedicated employees.  Check in was really easy and the front desk staff were very understanding and accommodating.  The room was very clean, the beds very comfortable, and the shower was spacious. Hallways and lobby were also spacious, very inviting, and modern.  The breakfast was and cut above the rest.  Food, cutlery, and condiments were nice.MoreShow less</t>
+  </si>
+  <si>
+    <t>July 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> traveled as a couple</t>
+  </si>
+  <si>
+    <t>Tony S, Director of Sales at Holiday Inn Hotel &amp; Suites Denver Tech Center-Centennial, responded to this reviewResponded 1 week ago</t>
+  </si>
+  <si>
+    <t>Responded 1 week ago</t>
+  </si>
+  <si>
+    <t>This is a beautiful facility well maintained by dedicated employees.  Check in was really easy and the front desk staff were very understanding and accommodating.  The room was very clean, the beds very comfortable, and the shower was spacious. Hallways and lobby were also spacious, very inviting, and modern.  The breakfast was and cut above the rest.  Food, cutlery, and condiments were nice.More</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r588955538-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>588955538</t>
+  </si>
+  <si>
+    <t>06/19/2018</t>
+  </si>
+  <si>
+    <t>Great place</t>
+  </si>
+  <si>
+    <t>The hotel is well maintained with clean rooms and a very friendly, helpful staff. The location is close to shopping and many restaurants. The hotel had a restaurant/bar located inside and an indoor pool.MoreShow less</t>
+  </si>
+  <si>
+    <t>May 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> traveled with family</t>
+  </si>
+  <si>
+    <t>Tony S, Director of Sales at Holiday Inn Hotel &amp; Suites Denver Tech Center-Centennial, responded to this reviewResponded June 20, 2018</t>
+  </si>
+  <si>
+    <t>Responded June 20, 2018</t>
+  </si>
+  <si>
+    <t>The hotel is well maintained with clean rooms and a very friendly, helpful staff. The location is close to shopping and many restaurants. The hotel had a restaurant/bar located inside and an indoor pool.More</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r588373329-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>588373329</t>
+  </si>
+  <si>
+    <t>06/18/2018</t>
+  </si>
+  <si>
+    <t>Top Notch Hotel!</t>
+  </si>
+  <si>
+    <t>I am the Manager of a Tour Company that uses hotels all across the country for over 250 nights each year.  The Holiday Inn Hotel &amp; Suites Denver Tech Center ranks as one of the top hotels that I have worked with.  From reservations to a smooth check-in process for my group to friendly and efficient staff while on the property - this hotel is just top notch.  The property is well-managed, clean, quiet, and comfortable, the nicely appointed rooms even have extra housekeeping touches and very comfortable beds.  This is my "go to" property in the Denver area.MoreShow less</t>
+  </si>
+  <si>
+    <t>June 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> traveled on business</t>
+  </si>
+  <si>
+    <t>Tony S, Director of Sales at Holiday Inn Hotel &amp; Suites Denver Tech Center-Centennial, responded to this reviewResponded June 19, 2018</t>
+  </si>
+  <si>
+    <t>Responded June 19, 2018</t>
+  </si>
+  <si>
+    <t>I am the Manager of a Tour Company that uses hotels all across the country for over 250 nights each year.  The Holiday Inn Hotel &amp; Suites Denver Tech Center ranks as one of the top hotels that I have worked with.  From reservations to a smooth check-in process for my group to friendly and efficient staff while on the property - this hotel is just top notch.  The property is well-managed, clean, quiet, and comfortable, the nicely appointed rooms even have extra housekeeping touches and very comfortable beds.  This is my "go to" property in the Denver area.More</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r557214054-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>557214054</t>
+  </si>
+  <si>
+    <t>01/29/2018</t>
+  </si>
+  <si>
+    <t>Great location and Staff!!</t>
+  </si>
+  <si>
+    <t>Had a wonderful stay here for a night out down south. Jeff was excellent on the check-in and going over the property amenities . Noticed it was very new and clean but the crazy carpet in the halls was trippy. Had some great beers on taps there at the small bar there ( Burger Theory was the name I think?) Karyn and Kerri were terrific and defiantly added a fun atmosphere to the place. I recommend swinging by for a visit even if your not staying there. Great overall experience. Looking forward to my next stay here!ChrisMoreShow less</t>
+  </si>
+  <si>
+    <t>December 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> traveled with friends</t>
+  </si>
+  <si>
+    <t>Tony S, Director of Sales at Holiday Inn Hotel &amp; Suites Denver Tech Center-Centennial, responded to this reviewResponded February 8, 2018</t>
+  </si>
+  <si>
+    <t>Responded February 8, 2018</t>
+  </si>
+  <si>
+    <t>Had a wonderful stay here for a night out down south. Jeff was excellent on the check-in and going over the property amenities . Noticed it was very new and clean but the crazy carpet in the halls was trippy. Had some great beers on taps there at the small bar there ( Burger Theory was the name I think?) Karyn and Kerri were terrific and defiantly added a fun atmosphere to the place. I recommend swinging by for a visit even if your not staying there. Great overall experience. Looking forward to my next stay here!ChrisMore</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r541683112-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>541683112</t>
+  </si>
+  <si>
+    <t>11/17/2017</t>
+  </si>
+  <si>
+    <t>Comfy beds in brand new DTC hotel</t>
+  </si>
+  <si>
+    <t>Stayed for a work event in Nov 2017.  The Holiday Inn had that "new building smell" and it seemed like some of the rooms had never been used.   The beds were very comfortable and the rooms were standard hotel fare.  No mini-bar (whatever) but did have a fridge.  The staff was excellent and very helpful and friendly. As others have mentioned, the water pressure was somewhat lackluster, but that's to be expected in Denver where water can be expensive.    Breakfast service left something to be desired, and one of my coworkers was late for a meeting because the food service was so slow.  The area is close for many business needs, but socially the place is a bit of a desert. There's plenty of parking, but no local shuttle bus so if you want to go out and drink, you'll need a DD or pay for an uber/lyft. Overall a good hotel for DTC business, but keep in mind there's not much around, so for fun you'll want to find a ride to the light rail.MoreShow less</t>
+  </si>
+  <si>
+    <t>November 2017</t>
+  </si>
+  <si>
+    <t>Stayed for a work event in Nov 2017.  The Holiday Inn had that "new building smell" and it seemed like some of the rooms had never been used.   The beds were very comfortable and the rooms were standard hotel fare.  No mini-bar (whatever) but did have a fridge.  The staff was excellent and very helpful and friendly. As others have mentioned, the water pressure was somewhat lackluster, but that's to be expected in Denver where water can be expensive.    Breakfast service left something to be desired, and one of my coworkers was late for a meeting because the food service was so slow.  The area is close for many business needs, but socially the place is a bit of a desert. There's plenty of parking, but no local shuttle bus so if you want to go out and drink, you'll need a DD or pay for an uber/lyft. Overall a good hotel for DTC business, but keep in mind there's not much around, so for fun you'll want to find a ride to the light rail.More</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r540398948-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>540398948</t>
+  </si>
+  <si>
+    <t>11/12/2017</t>
+  </si>
+  <si>
+    <t>Lovely new (1 year) hotel in a quiet area</t>
+  </si>
+  <si>
+    <t>Everything is clean and colorful - very modern and chic. Full bar with reasonable prices. Lovely rooms with comfortable beds and nice linens. Staff is very friendly and helpful. Plenty of free parking and easy access to freeways, shopping and restaurants.MoreShow less</t>
+  </si>
+  <si>
+    <t>Tony S, Director of Sales at Holiday Inn Hotel &amp; Suites Denver Tech Center-Centennial, responded to this reviewResponded November 13, 2017</t>
+  </si>
+  <si>
+    <t>Responded November 13, 2017</t>
+  </si>
+  <si>
+    <t>Everything is clean and colorful - very modern and chic. Full bar with reasonable prices. Lovely rooms with comfortable beds and nice linens. Staff is very friendly and helpful. Plenty of free parking and easy access to freeways, shopping and restaurants.More</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r531149066-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>531149066</t>
+  </si>
+  <si>
+    <t>10/08/2017</t>
+  </si>
+  <si>
+    <t>Very Nice</t>
+  </si>
+  <si>
+    <t>This is a new Holiday Inn. Very spacious rooms with large spansive windows. Although only a parking lot view in room 331. Bed was very comfortable. There is no breakfast but  many restaurant options in the area. I recommend Three Little Griddles not far away. There is a restaurant within the hotel called Burger Theory which has room service also.MoreShow less</t>
+  </si>
+  <si>
+    <t>September 2017</t>
+  </si>
+  <si>
+    <t>Tony S, Director of Sales at Holiday Inn Hotel &amp; Suites Denver Tech Center-Centennial, responded to this reviewResponded October 10, 2017</t>
+  </si>
+  <si>
+    <t>Responded October 10, 2017</t>
+  </si>
+  <si>
+    <t>This is a new Holiday Inn. Very spacious rooms with large spansive windows. Although only a parking lot view in room 331. Bed was very comfortable. There is no breakfast but  many restaurant options in the area. I recommend Three Little Griddles not far away. There is a restaurant within the hotel called Burger Theory which has room service also.More</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r527444627-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>527444627</t>
+  </si>
+  <si>
+    <t>09/25/2017</t>
+  </si>
+  <si>
+    <t>Excellent hotel</t>
+  </si>
+  <si>
+    <t>My husband and I came here due to hurricane Irma from Key Largo, FL. Tony, the manager, was amazing!  We feel that he really took care of us. He understood our situation and was very accommodating. All the staff was fantastic. It was clean and comfortable. Because of the destruction back in our hometown, we stayed almost 3 weeks. Every night, we would come back to our room saying, "home sweet hotel room!"  We will definitely come back. Thanks to all.MoreShow less</t>
+  </si>
+  <si>
+    <t>Tony S, Director of Sales at Holiday Inn Hotel &amp; Suites Denver Tech Center-Centennial, responded to this reviewResponded September 29, 2017</t>
+  </si>
+  <si>
+    <t>Responded September 29, 2017</t>
+  </si>
+  <si>
+    <t>My husband and I came here due to hurricane Irma from Key Largo, FL. Tony, the manager, was amazing!  We feel that he really took care of us. He understood our situation and was very accommodating. All the staff was fantastic. It was clean and comfortable. Because of the destruction back in our hometown, we stayed almost 3 weeks. Every night, we would come back to our room saying, "home sweet hotel room!"  We will definitely come back. Thanks to all.More</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r527436933-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>527436933</t>
+  </si>
+  <si>
+    <t>Great Hotel for your next Business Meeting</t>
+  </si>
+  <si>
+    <t>We booked a 2-day meeting with attendees coming from several different states.  Everyone loved the hotel, the food, and especially the comfortable beds.  The meeting room, snacks, and lunch were delicious.  Our hotel contact, Tony, took excellent care of us.  The event was a huge success with attendees saying it was one of the best venues they had attended.  Most of our attendees were without a car and appreciated having many dining options nearby.MoreShow less</t>
+  </si>
+  <si>
+    <t>We booked a 2-day meeting with attendees coming from several different states.  Everyone loved the hotel, the food, and especially the comfortable beds.  The meeting room, snacks, and lunch were delicious.  Our hotel contact, Tony, took excellent care of us.  The event was a huge success with attendees saying it was one of the best venues they had attended.  Most of our attendees were without a car and appreciated having many dining options nearby.More</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r507188762-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>507188762</t>
+  </si>
+  <si>
+    <t>07/30/2017</t>
+  </si>
+  <si>
+    <t>Really Nice Hotel</t>
+  </si>
+  <si>
+    <t>We got in late. the first room we walked into the a/c was making a really loud noise. So we switch room the hotel  was super nice about and felt bad about the a/c. the 2nd room was great. Very clean, its a brand new hotel. They had a restaurant we didn't eat they but our son did and love the food. We would go back againMoreShow less</t>
+  </si>
+  <si>
+    <t>July 2017</t>
+  </si>
+  <si>
+    <t>Tony S, Director of Sales at Holiday Inn Hotel &amp; Suites Denver Tech Center-Centennial, responded to this reviewResponded August 1, 2017</t>
+  </si>
+  <si>
+    <t>Responded August 1, 2017</t>
+  </si>
+  <si>
+    <t>We got in late. the first room we walked into the a/c was making a really loud noise. So we switch room the hotel  was super nice about and felt bad about the a/c. the 2nd room was great. Very clean, its a brand new hotel. They had a restaurant we didn't eat they but our son did and love the food. We would go back againMore</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r504429951-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>504429951</t>
+  </si>
+  <si>
+    <t>07/22/2017</t>
+  </si>
+  <si>
+    <t>Visit with Texas Friends</t>
+  </si>
+  <si>
+    <t>This should have been an easy 5 Stars as it is a new hotel, however...  The water pressure in the shower in 415 sucked. We told the desk and they said they had a plumber look at it, but no change over 2 day stay. It was like taking a shower in an RV. Desk personnel were as accommodating as they could be, providing us a few hotel bar coupons for our complaint. The room refrigerator was not plugged in...had to call maintenance to move the furniture to get it plugged in.  Lastly, only one towel in bathroom...had to call for more. I would try this place again as it might be growing pains...nice facilityMoreShow less</t>
+  </si>
+  <si>
+    <t>Tony S, Director of Sales at Holiday Inn Hotel &amp; Suites Denver Tech Center-Centennial, responded to this reviewResponded July 24, 2017</t>
+  </si>
+  <si>
+    <t>Responded July 24, 2017</t>
+  </si>
+  <si>
+    <t>This should have been an easy 5 Stars as it is a new hotel, however...  The water pressure in the shower in 415 sucked. We told the desk and they said they had a plumber look at it, but no change over 2 day stay. It was like taking a shower in an RV. Desk personnel were as accommodating as they could be, providing us a few hotel bar coupons for our complaint. The room refrigerator was not plugged in...had to call maintenance to move the furniture to get it plugged in.  Lastly, only one towel in bathroom...had to call for more. I would try this place again as it might be growing pains...nice facilityMore</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r502501432-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>502501432</t>
+  </si>
+  <si>
+    <t>07/16/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beautiful hotel </t>
+  </si>
+  <si>
+    <t>New hotel. Extremely clean and fresh look. Very well decorated. Comfortable beds and nice amenities. Would definitely stay again. Looks like a very new part of town. Kurig coffee maker in the room. Flat screen tv with directv and movie channels. MoreShow less</t>
+  </si>
+  <si>
+    <t>Tony S, Director of Sales at Holiday Inn Hotel &amp; Suites Denver Tech Center-Centennial, responded to this reviewResponded July 17, 2017</t>
+  </si>
+  <si>
+    <t>Responded July 17, 2017</t>
+  </si>
+  <si>
+    <t>New hotel. Extremely clean and fresh look. Very well decorated. Comfortable beds and nice amenities. Would definitely stay again. Looks like a very new part of town. Kurig coffee maker in the room. Flat screen tv with directv and movie channels. More</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r479599117-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>479599117</t>
+  </si>
+  <si>
+    <t>04/27/2017</t>
+  </si>
+  <si>
+    <t>We highly recommend this hotel!!!</t>
+  </si>
+  <si>
+    <t>My wife and I stayed here for 6 nights recently.  The rooms are spacious and comfortable.  I couldn't say enough about the beds...AMAZING!  The room was extremely clean when we checked in and housekeeping did a terrific job each and every day we stayed.The staff here truly made us feel like we were at home.  They greeted us with big hellos and smiles each time we walked through the hotel front doors.  I would stay here again just because of how great the staff was if for no other reason.The hotel has everything you could want...a pool, workout room, etc. Although we only ate in the restaurant once, the food was great and the service was as well just like the rest of the hotel staff.If you're ever looking for a hotel in the Denver area, you can't go wrong with this Holiday Inn.MoreShow less</t>
+  </si>
+  <si>
+    <t>April 2017</t>
+  </si>
+  <si>
+    <t>Tony S, Director of Sales at Holiday Inn Hotel &amp; Suites Denver Tech Center-Centennial, responded to this reviewResponded May 1, 2017</t>
+  </si>
+  <si>
+    <t>Responded May 1, 2017</t>
+  </si>
+  <si>
+    <t>My wife and I stayed here for 6 nights recently.  The rooms are spacious and comfortable.  I couldn't say enough about the beds...AMAZING!  The room was extremely clean when we checked in and housekeeping did a terrific job each and every day we stayed.The staff here truly made us feel like we were at home.  They greeted us with big hellos and smiles each time we walked through the hotel front doors.  I would stay here again just because of how great the staff was if for no other reason.The hotel has everything you could want...a pool, workout room, etc. Although we only ate in the restaurant once, the food was great and the service was as well just like the rest of the hotel staff.If you're ever looking for a hotel in the Denver area, you can't go wrong with this Holiday Inn.More</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r477118258-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>477118258</t>
+  </si>
+  <si>
+    <t>04/19/2017</t>
+  </si>
+  <si>
+    <t>Amazing people and not so amazing people</t>
+  </si>
+  <si>
+    <t>I travel a lot for business, which means I pretty much live in hotels. When I saw that there was a brand new just opened Holiday Inn I was so excited because the one I normally stay at is not so new not so great anymore. When I arrived I almost left, it was by far the LONGEST &amp; most disarray check in. 2 ladies was checking me in 1 was supposed to be a manager, I will not say their names cause I do not want to be cruel. They did not know what they were doing the lady who was not the manager had to be told multiple times on how to do something it was like watching a parent explain something to a toddler. My reservation was so messed up and was charged charges I should not have been. I was to frustrated and tired and just wanted to go to my room. Finally did after a very long 45 minute check in. After some rest I went to the front desk to straighten out the mess that was made on my reservation and there was a new lady at the desk. I was thinking great another one that will not know what she is doing. I explained what happened in a very annoyed mean tone. I will say her name because she was so wonderful. When I was done ranting she smiled at me and said...I travel a lot for business, which means I pretty much live in hotels. When I saw that there was a brand new just opened Holiday Inn I was so excited because the one I normally stay at is not so new not so great anymore. When I arrived I almost left, it was by far the LONGEST &amp; most disarray check in. 2 ladies was checking me in 1 was supposed to be a manager, I will not say their names cause I do not want to be cruel. They did not know what they were doing the lady who was not the manager had to be told multiple times on how to do something it was like watching a parent explain something to a toddler. My reservation was so messed up and was charged charges I should not have been. I was to frustrated and tired and just wanted to go to my room. Finally did after a very long 45 minute check in. After some rest I went to the front desk to straighten out the mess that was made on my reservation and there was a new lady at the desk. I was thinking great another one that will not know what she is doing. I explained what happened in a very annoyed mean tone. I will say her name because she was so wonderful. When I was done ranting she smiled at me and said ma'am I sincerely apologize for the experience you have had. She then fixed EVERYTHING in a matter of a few minutes, she comped a snack and drink from there store and gave me extra points for the bad experience. She then apologized again as if it was her mistake which it was not. She told me to let her know if there was anything else to please let her know, and that if in the morning when she was not there to talk to her son and he would take good care of me. The next day I did have a small issue and was thinking I wish she was here cause I do not want to have to explain everything all over. I went to the desk and the young man knew everything already the night lady had already told him about it. He took good care of me and said if I needed anything else to let him know. I started out with a very bad experience and these 2 mother and son duo made it amazing. I will return only because of these 2. I hope that management know what amazing 2 workers they have. Thank you Catina and Cody for making a bad experience turn into a wonderful experience. You 2 are the reason I am giving 5 stars.MoreShow less</t>
+  </si>
+  <si>
+    <t>Tony S, Director of Sales at Holiday Inn Hotel &amp; Suites Denver Tech Center-Centennial, responded to this reviewResponded June 24, 2017</t>
+  </si>
+  <si>
+    <t>Responded June 24, 2017</t>
+  </si>
+  <si>
+    <t>I travel a lot for business, which means I pretty much live in hotels. When I saw that there was a brand new just opened Holiday Inn I was so excited because the one I normally stay at is not so new not so great anymore. When I arrived I almost left, it was by far the LONGEST &amp; most disarray check in. 2 ladies was checking me in 1 was supposed to be a manager, I will not say their names cause I do not want to be cruel. They did not know what they were doing the lady who was not the manager had to be told multiple times on how to do something it was like watching a parent explain something to a toddler. My reservation was so messed up and was charged charges I should not have been. I was to frustrated and tired and just wanted to go to my room. Finally did after a very long 45 minute check in. After some rest I went to the front desk to straighten out the mess that was made on my reservation and there was a new lady at the desk. I was thinking great another one that will not know what she is doing. I explained what happened in a very annoyed mean tone. I will say her name because she was so wonderful. When I was done ranting she smiled at me and said...I travel a lot for business, which means I pretty much live in hotels. When I saw that there was a brand new just opened Holiday Inn I was so excited because the one I normally stay at is not so new not so great anymore. When I arrived I almost left, it was by far the LONGEST &amp; most disarray check in. 2 ladies was checking me in 1 was supposed to be a manager, I will not say their names cause I do not want to be cruel. They did not know what they were doing the lady who was not the manager had to be told multiple times on how to do something it was like watching a parent explain something to a toddler. My reservation was so messed up and was charged charges I should not have been. I was to frustrated and tired and just wanted to go to my room. Finally did after a very long 45 minute check in. After some rest I went to the front desk to straighten out the mess that was made on my reservation and there was a new lady at the desk. I was thinking great another one that will not know what she is doing. I explained what happened in a very annoyed mean tone. I will say her name because she was so wonderful. When I was done ranting she smiled at me and said ma'am I sincerely apologize for the experience you have had. She then fixed EVERYTHING in a matter of a few minutes, she comped a snack and drink from there store and gave me extra points for the bad experience. She then apologized again as if it was her mistake which it was not. She told me to let her know if there was anything else to please let her know, and that if in the morning when she was not there to talk to her son and he would take good care of me. The next day I did have a small issue and was thinking I wish she was here cause I do not want to have to explain everything all over. I went to the desk and the young man knew everything already the night lady had already told him about it. He took good care of me and said if I needed anything else to let him know. I started out with a very bad experience and these 2 mother and son duo made it amazing. I will return only because of these 2. I hope that management know what amazing 2 workers they have. Thank you Catina and Cody for making a bad experience turn into a wonderful experience. You 2 are the reason I am giving 5 stars.More</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowUserReviews-g609128-d10190804-r473484067-Holiday_Inn_Hotel_Suites_Denver_Tech_Center_Centennial-Centennial_Colorado.html</t>
+  </si>
+  <si>
+    <t>473484067</t>
+  </si>
+  <si>
+    <t>04/07/2017</t>
+  </si>
+  <si>
+    <t>Amasing.....</t>
+  </si>
+  <si>
+    <t>Beautiful hotel all new. Staff very attentive and helpful. The maids very attentive and with the correct answers to our questions. The cleanliness unbeatable. Without doubts I will return ...... I love this hotelMoreShow less</t>
+  </si>
+  <si>
+    <t>Tony S, Director of Sales at Holiday Inn Hotel &amp; Suites Denver Tech Center-Centennial, responded to this reviewResponded April 9, 2017</t>
+  </si>
+  <si>
+    <t>Responded April 9, 2017</t>
+  </si>
+  <si>
+    <t>Beautiful hotel all new. Staff very attentive and helpful. The maids very attentive and with the correct answers to our questions. The cleanliness unbeatable. Without doubts I will return ...... I love this hotelMore</t>
   </si>
 </sst>
 </file>
@@ -532,11 +928,17 @@
       <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s"/>
-      <c r="H2" t="s"/>
-      <c r="I2" t="s"/>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -558,79 +960,1026 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="O1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Q1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="S1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="U1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="V1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="W1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="X1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Y1" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B2" t="s"/>
+      <c r="C2" t="s"/>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" t="n">
+        <v>5</v>
+      </c>
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" t="s"/>
+      <c r="Q2" t="s"/>
+      <c r="R2" t="s"/>
+      <c r="S2" t="s"/>
+      <c r="T2" t="s"/>
+      <c r="U2" t="s"/>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B3" t="s"/>
+      <c r="C3" t="s"/>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" t="n">
+        <v>4</v>
+      </c>
+      <c r="N3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P3" t="s"/>
+      <c r="Q3" t="s"/>
+      <c r="R3" t="s"/>
+      <c r="S3" t="s"/>
+      <c r="T3" t="s"/>
+      <c r="U3" t="s"/>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B4" t="s"/>
+      <c r="C4" t="s"/>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" t="s">
+        <v>72</v>
+      </c>
+      <c r="P4" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>5</v>
+      </c>
+      <c r="R4" t="s"/>
+      <c r="S4" t="s"/>
+      <c r="T4" t="s"/>
+      <c r="U4" t="n">
+        <v>5</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="s">
+        <v>73</v>
+      </c>
+      <c r="X4" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B5" t="s"/>
+      <c r="C5" t="s"/>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" t="n">
+        <v>5</v>
+      </c>
+      <c r="N5" t="s">
+        <v>81</v>
+      </c>
+      <c r="O5" t="s">
+        <v>82</v>
+      </c>
+      <c r="P5" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q5" t="s"/>
+      <c r="R5" t="s"/>
+      <c r="S5" t="s"/>
+      <c r="T5" t="s"/>
+      <c r="U5" t="n">
+        <v>5</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="s">
+        <v>83</v>
+      </c>
+      <c r="X5" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B6" t="s"/>
+      <c r="C6" t="s"/>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" t="s">
+        <v>89</v>
+      </c>
+      <c r="L6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M6" t="n">
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
+        <v>91</v>
+      </c>
+      <c r="O6" t="s">
+        <v>72</v>
+      </c>
+      <c r="P6" t="s"/>
+      <c r="Q6" t="n">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s"/>
+      <c r="S6" t="s"/>
+      <c r="T6" t="s"/>
+      <c r="U6" t="n">
+        <v>4</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="s"/>
+      <c r="X6" t="s"/>
+      <c r="Y6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B7" t="s"/>
+      <c r="C7" t="s"/>
+      <c r="D7" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" t="s">
+        <v>95</v>
+      </c>
+      <c r="K7" t="s">
+        <v>96</v>
+      </c>
+      <c r="L7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M7" t="n">
+        <v>5</v>
+      </c>
+      <c r="N7" t="s">
+        <v>91</v>
+      </c>
+      <c r="O7" t="s">
+        <v>82</v>
+      </c>
+      <c r="P7" t="s"/>
+      <c r="Q7" t="s"/>
+      <c r="R7" t="s"/>
+      <c r="S7" t="s"/>
+      <c r="T7" t="s"/>
+      <c r="U7" t="s"/>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="s">
+        <v>98</v>
+      </c>
+      <c r="X7" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B8" t="s"/>
+      <c r="C8" t="s"/>
+      <c r="D8" t="n">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J8" t="s">
+        <v>103</v>
+      </c>
+      <c r="K8" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" t="s">
+        <v>105</v>
+      </c>
+      <c r="M8" t="n">
+        <v>4</v>
+      </c>
+      <c r="N8" t="s">
+        <v>106</v>
+      </c>
+      <c r="O8" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>4</v>
+      </c>
+      <c r="R8" t="s"/>
+      <c r="S8" t="s"/>
+      <c r="T8" t="s"/>
+      <c r="U8" t="n">
+        <v>4</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="s">
+        <v>107</v>
+      </c>
+      <c r="X8" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B9" t="s"/>
+      <c r="C9" t="s"/>
+      <c r="D9" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" t="s">
+        <v>111</v>
+      </c>
+      <c r="J9" t="s">
+        <v>112</v>
+      </c>
+      <c r="K9" t="s">
+        <v>113</v>
+      </c>
+      <c r="L9" t="s">
+        <v>114</v>
+      </c>
+      <c r="M9" t="n">
+        <v>5</v>
+      </c>
+      <c r="N9" t="s">
+        <v>106</v>
+      </c>
+      <c r="O9" t="s">
+        <v>62</v>
+      </c>
+      <c r="P9" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q9" t="s"/>
+      <c r="R9" t="s"/>
+      <c r="S9" t="s"/>
+      <c r="T9" t="s"/>
+      <c r="U9" t="n">
+        <v>5</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="s">
+        <v>115</v>
+      </c>
+      <c r="X9" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B10" t="s"/>
+      <c r="C10" t="s"/>
+      <c r="D10" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" t="s">
+        <v>119</v>
+      </c>
+      <c r="J10" t="s">
+        <v>112</v>
+      </c>
+      <c r="K10" t="s">
+        <v>120</v>
+      </c>
+      <c r="L10" t="s">
+        <v>121</v>
+      </c>
+      <c r="M10" t="n">
+        <v>5</v>
+      </c>
+      <c r="N10" t="s">
+        <v>106</v>
+      </c>
+      <c r="O10" t="s">
+        <v>72</v>
+      </c>
+      <c r="P10" t="s"/>
+      <c r="Q10" t="s"/>
+      <c r="R10" t="s"/>
+      <c r="S10" t="s"/>
+      <c r="T10" t="s"/>
+      <c r="U10" t="s"/>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" t="s">
+        <v>115</v>
+      </c>
+      <c r="X10" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B11" t="s"/>
+      <c r="C11" t="s"/>
+      <c r="D11" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" t="s">
+        <v>124</v>
+      </c>
+      <c r="J11" t="s">
+        <v>125</v>
+      </c>
+      <c r="K11" t="s">
+        <v>126</v>
+      </c>
+      <c r="L11" t="s">
+        <v>127</v>
+      </c>
+      <c r="M11" t="n">
+        <v>5</v>
+      </c>
+      <c r="N11" t="s">
+        <v>128</v>
+      </c>
+      <c r="O11" t="s">
+        <v>62</v>
+      </c>
+      <c r="P11" t="s"/>
+      <c r="Q11" t="n">
+        <v>5</v>
+      </c>
+      <c r="R11" t="s"/>
+      <c r="S11" t="n">
+        <v>5</v>
+      </c>
+      <c r="T11" t="s"/>
+      <c r="U11" t="n">
+        <v>5</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="s">
+        <v>129</v>
+      </c>
+      <c r="X11" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B12" t="s"/>
+      <c r="C12" t="s"/>
+      <c r="D12" t="n">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" t="s">
+        <v>133</v>
+      </c>
+      <c r="J12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L12" t="s">
+        <v>136</v>
+      </c>
+      <c r="M12" t="n">
+        <v>4</v>
+      </c>
+      <c r="N12" t="s"/>
+      <c r="O12" t="s"/>
+      <c r="P12" t="s"/>
+      <c r="Q12" t="s"/>
+      <c r="R12" t="s"/>
+      <c r="S12" t="s"/>
+      <c r="T12" t="s"/>
+      <c r="U12" t="s"/>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="s">
+        <v>137</v>
+      </c>
+      <c r="X12" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B13" t="s"/>
+      <c r="C13" t="s"/>
+      <c r="D13" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>140</v>
+      </c>
+      <c r="G13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" t="s">
+        <v>141</v>
+      </c>
+      <c r="J13" t="s">
+        <v>142</v>
+      </c>
+      <c r="K13" t="s">
+        <v>143</v>
+      </c>
+      <c r="L13" t="s">
+        <v>144</v>
+      </c>
+      <c r="M13" t="n">
+        <v>5</v>
+      </c>
+      <c r="N13" t="s">
+        <v>128</v>
+      </c>
+      <c r="O13" t="s">
+        <v>82</v>
+      </c>
+      <c r="P13" t="s"/>
+      <c r="Q13" t="s"/>
+      <c r="R13" t="s"/>
+      <c r="S13" t="s"/>
+      <c r="T13" t="s"/>
+      <c r="U13" t="s"/>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="s">
+        <v>145</v>
+      </c>
+      <c r="X13" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B14" t="s"/>
+      <c r="C14" t="s"/>
+      <c r="D14" t="n">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>148</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" t="s">
+        <v>149</v>
+      </c>
+      <c r="J14" t="s">
+        <v>150</v>
+      </c>
+      <c r="K14" t="s">
+        <v>151</v>
+      </c>
+      <c r="L14" t="s">
+        <v>152</v>
+      </c>
+      <c r="M14" t="n">
+        <v>5</v>
+      </c>
+      <c r="N14" t="s">
+        <v>153</v>
+      </c>
+      <c r="O14" t="s">
+        <v>52</v>
+      </c>
+      <c r="P14" t="s"/>
+      <c r="Q14" t="s"/>
+      <c r="R14" t="s"/>
+      <c r="S14" t="n">
+        <v>5</v>
+      </c>
+      <c r="T14" t="s"/>
+      <c r="U14" t="n">
+        <v>5</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" t="s">
+        <v>154</v>
+      </c>
+      <c r="X14" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B15" t="s"/>
+      <c r="C15" t="s"/>
+      <c r="D15" t="n">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>157</v>
+      </c>
+      <c r="G15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" t="s">
+        <v>158</v>
+      </c>
+      <c r="J15" t="s">
+        <v>159</v>
+      </c>
+      <c r="K15" t="s">
+        <v>160</v>
+      </c>
+      <c r="L15" t="s">
+        <v>161</v>
+      </c>
+      <c r="M15" t="n">
+        <v>5</v>
+      </c>
+      <c r="N15" t="s">
+        <v>153</v>
+      </c>
+      <c r="O15" t="s">
+        <v>72</v>
+      </c>
+      <c r="P15" t="s"/>
+      <c r="Q15" t="s"/>
+      <c r="R15" t="s"/>
+      <c r="S15" t="s"/>
+      <c r="T15" t="s"/>
+      <c r="U15" t="s"/>
+      <c r="V15" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" t="s">
+        <v>162</v>
+      </c>
+      <c r="X15" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>65503</v>
+      </c>
+      <c r="B16" t="s"/>
+      <c r="C16" t="s"/>
+      <c r="D16" t="n">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>165</v>
+      </c>
+      <c r="G16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J16" t="s">
+        <v>167</v>
+      </c>
+      <c r="K16" t="s">
+        <v>168</v>
+      </c>
+      <c r="L16" t="s">
+        <v>169</v>
+      </c>
+      <c r="M16" t="n">
+        <v>5</v>
+      </c>
+      <c r="N16" t="s">
+        <v>153</v>
+      </c>
+      <c r="O16" t="s">
+        <v>72</v>
+      </c>
+      <c r="P16" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q16" t="s"/>
+      <c r="R16" t="n">
+        <v>5</v>
+      </c>
+      <c r="S16" t="s"/>
+      <c r="T16" t="s"/>
+      <c r="U16" t="n">
+        <v>5</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="s">
+        <v>170</v>
+      </c>
+      <c r="X16" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>